<commit_message>
Working version with power adjusted control
</commit_message>
<xml_diff>
--- a/misc/calcs/ESC-ISR.xlsx
+++ b/misc/calcs/ESC-ISR.xlsx
@@ -9,13 +9,12 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="11370" windowHeight="6045"/>
+    <workbookView minimized="1" xWindow="0" yWindow="0" windowWidth="11370" windowHeight="6045"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="152511"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -25,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="250" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="236" uniqueCount="36">
   <si>
     <t>START</t>
   </si>
@@ -124,6 +123,15 @@
   </si>
   <si>
     <t>LATENCY IF TO OFF</t>
+  </si>
+  <si>
+    <t>A</t>
+  </si>
+  <si>
+    <t>B</t>
+  </si>
+  <si>
+    <t>C</t>
   </si>
 </sst>
 </file>
@@ -552,7 +560,7 @@
   <dimension ref="A1:L226"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A200" workbookViewId="0">
-      <selection activeCell="E212" sqref="E212"/>
+      <selection activeCell="E210" sqref="E210"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4154,20 +4162,16 @@
     </row>
     <row r="210" spans="4:10" x14ac:dyDescent="0.25">
       <c r="D210" t="s">
-        <v>0</v>
-      </c>
-      <c r="E210" s="10">
-        <v>2369.19</v>
-      </c>
+        <v>33</v>
+      </c>
+      <c r="E210" s="10"/>
       <c r="F210" s="11">
         <v>0</v>
       </c>
-      <c r="G210" s="10">
-        <v>32</v>
-      </c>
+      <c r="G210" s="10"/>
       <c r="H210" s="11">
         <f>(G210/16000000)*1000000</f>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="I210" s="10"/>
       <c r="J210" s="11">
@@ -4177,21 +4181,17 @@
     </row>
     <row r="211" spans="4:10" x14ac:dyDescent="0.25">
       <c r="D211" t="s">
-        <v>5</v>
-      </c>
-      <c r="E211" s="10">
-        <v>2702.19</v>
-      </c>
+        <v>34</v>
+      </c>
+      <c r="E211" s="10"/>
       <c r="F211" s="11">
         <f t="shared" ref="F211:F226" si="33">E211-E210</f>
-        <v>333</v>
-      </c>
-      <c r="G211" s="10">
-        <v>968</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="G211" s="10"/>
       <c r="H211" s="11">
         <f t="shared" ref="H211:H226" si="34">(G211/16000000)*1000000</f>
-        <v>60.5</v>
+        <v>0</v>
       </c>
       <c r="I211" s="10"/>
       <c r="J211" s="11">
@@ -4201,19 +4201,17 @@
     </row>
     <row r="212" spans="4:10" x14ac:dyDescent="0.25">
       <c r="D212" t="s">
-        <v>6</v>
+        <v>35</v>
       </c>
       <c r="E212" s="10"/>
       <c r="F212" s="11">
         <f t="shared" si="33"/>
-        <v>-2702.19</v>
-      </c>
-      <c r="G212" s="10">
-        <v>32</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="G212" s="10"/>
       <c r="H212" s="11">
         <f t="shared" si="34"/>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="I212" s="10"/>
       <c r="J212" s="11">
@@ -4222,20 +4220,15 @@
       </c>
     </row>
     <row r="213" spans="4:10" x14ac:dyDescent="0.25">
-      <c r="D213" t="s">
-        <v>1</v>
-      </c>
       <c r="E213" s="10"/>
       <c r="F213" s="11">
         <f t="shared" si="33"/>
         <v>0</v>
       </c>
-      <c r="G213" s="10">
-        <v>7163</v>
-      </c>
+      <c r="G213" s="10"/>
       <c r="H213" s="11">
         <f t="shared" si="34"/>
-        <v>447.6875</v>
+        <v>0</v>
       </c>
       <c r="I213" s="10"/>
       <c r="J213" s="11">
@@ -4244,20 +4237,15 @@
       </c>
     </row>
     <row r="214" spans="4:10" x14ac:dyDescent="0.25">
-      <c r="D214" t="s">
-        <v>2</v>
-      </c>
       <c r="E214" s="10"/>
       <c r="F214" s="11">
         <f t="shared" si="33"/>
         <v>0</v>
       </c>
-      <c r="G214" s="10">
-        <v>32</v>
-      </c>
+      <c r="G214" s="10"/>
       <c r="H214" s="11">
         <f t="shared" si="34"/>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="I214" s="10"/>
       <c r="J214" s="11">
@@ -4266,20 +4254,15 @@
       </c>
     </row>
     <row r="215" spans="4:10" x14ac:dyDescent="0.25">
-      <c r="D215" t="s">
-        <v>3</v>
-      </c>
       <c r="E215" s="10"/>
       <c r="F215" s="11">
         <f t="shared" si="33"/>
         <v>0</v>
       </c>
-      <c r="G215" s="10">
-        <v>6599</v>
-      </c>
+      <c r="G215" s="10"/>
       <c r="H215" s="11">
         <f t="shared" si="34"/>
-        <v>412.4375</v>
+        <v>0</v>
       </c>
       <c r="I215" s="10"/>
       <c r="J215" s="11">
@@ -4288,20 +4271,15 @@
       </c>
     </row>
     <row r="216" spans="4:10" x14ac:dyDescent="0.25">
-      <c r="D216" t="s">
-        <v>4</v>
-      </c>
       <c r="E216" s="10"/>
       <c r="F216" s="11">
         <f t="shared" si="33"/>
         <v>0</v>
       </c>
-      <c r="G216" s="10">
-        <v>32</v>
-      </c>
+      <c r="G216" s="10"/>
       <c r="H216" s="11">
         <f t="shared" si="34"/>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="I216" s="10"/>
       <c r="J216" s="11">
@@ -4310,20 +4288,15 @@
       </c>
     </row>
     <row r="217" spans="4:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D217" t="s">
-        <v>7</v>
-      </c>
       <c r="E217" s="12"/>
       <c r="F217" s="13">
         <f t="shared" si="33"/>
         <v>0</v>
       </c>
-      <c r="G217" s="12">
-        <v>1110</v>
-      </c>
+      <c r="G217" s="12"/>
       <c r="H217" s="13">
         <f t="shared" si="34"/>
-        <v>69.375</v>
+        <v>0</v>
       </c>
       <c r="I217" s="12"/>
       <c r="J217" s="13">
@@ -4332,20 +4305,15 @@
       </c>
     </row>
     <row r="218" spans="4:10" x14ac:dyDescent="0.25">
-      <c r="D218" t="s">
-        <v>0</v>
-      </c>
       <c r="E218" s="10"/>
       <c r="F218" s="11">
         <f t="shared" si="33"/>
         <v>0</v>
       </c>
-      <c r="G218" s="10">
-        <v>32</v>
-      </c>
+      <c r="G218" s="10"/>
       <c r="H218" s="11">
         <f t="shared" si="34"/>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="I218" s="10"/>
       <c r="J218" s="11">
@@ -4354,20 +4322,15 @@
       </c>
     </row>
     <row r="219" spans="4:10" x14ac:dyDescent="0.25">
-      <c r="D219" t="s">
-        <v>5</v>
-      </c>
       <c r="E219" s="10"/>
       <c r="F219" s="11">
         <f t="shared" si="33"/>
         <v>0</v>
       </c>
-      <c r="G219" s="10">
-        <v>593</v>
-      </c>
+      <c r="G219" s="10"/>
       <c r="H219" s="11">
         <f t="shared" si="34"/>
-        <v>37.0625</v>
+        <v>0</v>
       </c>
       <c r="I219" s="10"/>
       <c r="J219" s="11">
@@ -4376,137 +4339,102 @@
       </c>
     </row>
     <row r="220" spans="4:10" x14ac:dyDescent="0.25">
-      <c r="D220" t="s">
-        <v>6</v>
-      </c>
       <c r="E220" s="10"/>
       <c r="F220" s="11">
         <f t="shared" si="33"/>
         <v>0</v>
       </c>
-      <c r="G220" s="10">
-        <v>32</v>
-      </c>
+      <c r="G220" s="10"/>
       <c r="H220" s="11">
         <f t="shared" si="34"/>
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="221" spans="4:10" x14ac:dyDescent="0.25">
-      <c r="D221" t="s">
-        <v>1</v>
-      </c>
       <c r="E221" s="10"/>
       <c r="F221" s="11">
         <f t="shared" si="33"/>
         <v>0</v>
       </c>
-      <c r="G221" s="14">
-        <v>8289</v>
-      </c>
+      <c r="G221" s="14"/>
       <c r="H221" s="11">
         <f t="shared" si="34"/>
-        <v>518.0625</v>
+        <v>0</v>
       </c>
     </row>
     <row r="222" spans="4:10" x14ac:dyDescent="0.25">
-      <c r="D222" t="s">
-        <v>2</v>
-      </c>
       <c r="E222" s="10"/>
       <c r="F222" s="11">
         <f t="shared" si="33"/>
         <v>0</v>
       </c>
-      <c r="G222" s="14">
-        <v>32</v>
-      </c>
+      <c r="G222" s="14"/>
       <c r="H222" s="11">
         <f t="shared" si="34"/>
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="223" spans="4:10" x14ac:dyDescent="0.25">
-      <c r="D223" t="s">
-        <v>3</v>
-      </c>
       <c r="E223" s="10"/>
       <c r="F223" s="11">
         <f t="shared" si="33"/>
         <v>0</v>
       </c>
-      <c r="G223" s="14">
-        <v>5411</v>
-      </c>
+      <c r="G223" s="14"/>
       <c r="H223" s="11">
         <f t="shared" si="34"/>
-        <v>338.1875</v>
+        <v>0</v>
       </c>
     </row>
     <row r="224" spans="4:10" x14ac:dyDescent="0.25">
-      <c r="D224" t="s">
-        <v>4</v>
-      </c>
       <c r="E224" s="10"/>
       <c r="F224" s="11">
         <f t="shared" si="33"/>
         <v>0</v>
       </c>
-      <c r="G224" s="14">
-        <v>32</v>
-      </c>
+      <c r="G224" s="14"/>
       <c r="H224" s="11">
         <f t="shared" si="34"/>
-        <v>2</v>
-      </c>
-    </row>
-    <row r="225" spans="4:8" x14ac:dyDescent="0.25">
-      <c r="D225" t="s">
-        <v>7</v>
-      </c>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="225" spans="5:8" x14ac:dyDescent="0.25">
       <c r="E225" s="10"/>
       <c r="F225" s="11">
         <f t="shared" si="33"/>
         <v>0</v>
       </c>
-      <c r="G225" s="14">
-        <v>1547</v>
-      </c>
+      <c r="G225" s="14"/>
       <c r="H225" s="11">
         <f t="shared" si="34"/>
-        <v>96.6875</v>
-      </c>
-    </row>
-    <row r="226" spans="4:8" x14ac:dyDescent="0.25">
-      <c r="D226" t="s">
-        <v>0</v>
-      </c>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="226" spans="5:8" x14ac:dyDescent="0.25">
       <c r="E226" s="10"/>
       <c r="F226" s="11">
         <f t="shared" si="33"/>
         <v>0</v>
       </c>
-      <c r="G226" s="14">
-        <v>32</v>
-      </c>
+      <c r="G226" s="14"/>
       <c r="H226" s="11">
         <f t="shared" si="34"/>
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="11">
-    <mergeCell ref="F2:G2"/>
-    <mergeCell ref="F18:G18"/>
-    <mergeCell ref="F34:G34"/>
-    <mergeCell ref="F49:G49"/>
-    <mergeCell ref="F64:G64"/>
     <mergeCell ref="F131:G131"/>
     <mergeCell ref="F150:G150"/>
     <mergeCell ref="F171:G171"/>
     <mergeCell ref="E208:F208"/>
     <mergeCell ref="F83:G83"/>
     <mergeCell ref="F102:G102"/>
+    <mergeCell ref="F2:G2"/>
+    <mergeCell ref="F18:G18"/>
+    <mergeCell ref="F34:G34"/>
+    <mergeCell ref="F49:G49"/>
+    <mergeCell ref="F64:G64"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>